<commit_message>
22.04.19 Sales Updated 10:45Pm
</commit_message>
<xml_diff>
--- a/Othes/Allocation Sheet.xlsx
+++ b/Othes/Allocation Sheet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="330" windowWidth="19875" windowHeight="7710"/>
@@ -13,7 +13,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Running!$A$5:$A$136</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Running!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -311,13 +311,13 @@
     <t>Delivered By</t>
   </si>
   <si>
-    <t>Date:21.04.19</t>
-  </si>
-  <si>
     <t>Amount</t>
   </si>
   <si>
     <t>v128</t>
+  </si>
+  <si>
+    <t>Date:22.04.19</t>
   </si>
 </sst>
 </file>
@@ -603,15 +603,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -619,15 +610,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="18" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -637,47 +619,65 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1073,8 +1073,8 @@
   </sheetPr>
   <dimension ref="A1:S134"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection sqref="A1:M61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="12.75"/>
@@ -1094,21 +1094,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="23.25" customHeight="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -1117,21 +1117,21 @@
       <c r="S1" s="4"/>
     </row>
     <row r="2" spans="1:19" ht="16.5" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -1140,21 +1140,21 @@
       <c r="S2" s="5"/>
     </row>
     <row r="3" spans="1:19" ht="18.75" customHeight="1">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="44"/>
+      <c r="K3" s="44"/>
+      <c r="L3" s="44"/>
+      <c r="M3" s="44"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
@@ -1163,21 +1163,21 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A4" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
+      <c r="A4" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
@@ -1186,41 +1186,41 @@
       <c r="S4" s="6"/>
     </row>
     <row r="5" spans="1:19" ht="16.5" customHeight="1" thickTop="1">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="26" t="s">
+      <c r="F5" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="24"/>
+      <c r="H5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="27" t="s">
+      <c r="K5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="27" t="s">
+      <c r="L5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="27" t="s">
+      <c r="M5" s="24" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1236,7 +1236,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="34" t="s">
         <v>69</v>
       </c>
       <c r="I6" s="14">
@@ -1259,7 +1259,7 @@
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="45" t="s">
+      <c r="H7" s="35" t="s">
         <v>91</v>
       </c>
       <c r="I7" s="20">
@@ -1328,7 +1328,7 @@
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="45" t="s">
+      <c r="H10" s="35" t="s">
         <v>49</v>
       </c>
       <c r="I10" s="14">
@@ -1351,7 +1351,7 @@
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
-      <c r="H11" s="45" t="s">
+      <c r="H11" s="35" t="s">
         <v>92</v>
       </c>
       <c r="I11" s="14">
@@ -1397,7 +1397,7 @@
       <c r="E13" s="17"/>
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="44" t="s">
+      <c r="H13" s="34" t="s">
         <v>59</v>
       </c>
       <c r="I13" s="14">
@@ -1443,7 +1443,7 @@
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
-      <c r="H15" s="44" t="s">
+      <c r="H15" s="34" t="s">
         <v>60</v>
       </c>
       <c r="I15" s="14">
@@ -1466,7 +1466,7 @@
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
-      <c r="H16" s="44" t="s">
+      <c r="H16" s="34" t="s">
         <v>19</v>
       </c>
       <c r="I16" s="14">
@@ -1535,7 +1535,7 @@
       <c r="E19" s="17"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="34" t="s">
         <v>40</v>
       </c>
       <c r="I19" s="14">
@@ -1582,7 +1582,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
       <c r="H21" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I21" s="14">
         <v>4640</v>
@@ -1719,7 +1719,7 @@
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
-      <c r="H27" s="45" t="s">
+      <c r="H27" s="35" t="s">
         <v>58</v>
       </c>
       <c r="I27" s="14">
@@ -1742,7 +1742,7 @@
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
-      <c r="H28" s="45" t="s">
+      <c r="H28" s="35" t="s">
         <v>43</v>
       </c>
       <c r="I28" s="14">
@@ -1788,7 +1788,7 @@
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
-      <c r="H30" s="44" t="s">
+      <c r="H30" s="34" t="s">
         <v>83</v>
       </c>
       <c r="I30" s="20">
@@ -1811,7 +1811,7 @@
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
       <c r="G31" s="17"/>
-      <c r="H31" s="44" t="s">
+      <c r="H31" s="34" t="s">
         <v>84</v>
       </c>
       <c r="I31" s="20">
@@ -1834,7 +1834,7 @@
       <c r="E32" s="17"/>
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
-      <c r="H32" s="44" t="s">
+      <c r="H32" s="34" t="s">
         <v>85</v>
       </c>
       <c r="I32" s="14">
@@ -1903,7 +1903,7 @@
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
-      <c r="H35" s="44" t="s">
+      <c r="H35" s="34" t="s">
         <v>88</v>
       </c>
       <c r="I35" s="14">
@@ -1926,7 +1926,7 @@
       <c r="E36" s="17"/>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
-      <c r="H36" s="44" t="s">
+      <c r="H36" s="34" t="s">
         <v>89</v>
       </c>
       <c r="I36" s="14">
@@ -1949,7 +1949,7 @@
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
-      <c r="H37" s="44"/>
+      <c r="H37" s="34"/>
       <c r="I37" s="14"/>
       <c r="J37" s="17"/>
       <c r="K37" s="17"/>
@@ -1968,7 +1968,7 @@
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
-      <c r="H38" s="44"/>
+      <c r="H38" s="34"/>
       <c r="I38" s="14"/>
       <c r="J38" s="17"/>
       <c r="K38" s="17"/>
@@ -2006,7 +2006,7 @@
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
-      <c r="H40" s="45"/>
+      <c r="H40" s="35"/>
       <c r="I40" s="14"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
@@ -2025,7 +2025,7 @@
       <c r="E41" s="17"/>
       <c r="F41" s="17"/>
       <c r="G41" s="17"/>
-      <c r="H41" s="45"/>
+      <c r="H41" s="35"/>
       <c r="I41" s="14"/>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
@@ -2044,7 +2044,7 @@
       <c r="E42" s="17"/>
       <c r="F42" s="17"/>
       <c r="G42" s="17"/>
-      <c r="H42" s="45"/>
+      <c r="H42" s="35"/>
       <c r="I42" s="14"/>
       <c r="J42" s="17"/>
       <c r="K42" s="17"/>
@@ -2063,14 +2063,14 @@
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
       <c r="G43" s="17"/>
-      <c r="H43" s="29" t="s">
+      <c r="H43" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="I43" s="46"/>
+      <c r="I43" s="50"/>
       <c r="J43" s="22"/>
-      <c r="K43" s="29"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="43"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="33"/>
     </row>
     <row r="44" spans="1:13" ht="16.5" customHeight="1">
       <c r="A44" s="12" t="s">
@@ -2084,12 +2084,12 @@
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
-      <c r="H44" s="29"/>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
-      <c r="K44" s="29"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="29"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
     </row>
     <row r="45" spans="1:13" ht="16.5" customHeight="1">
       <c r="A45" s="12" t="s">
@@ -2110,7 +2110,7 @@
       <c r="J45" s="47"/>
       <c r="K45" s="47"/>
       <c r="L45" s="47"/>
-      <c r="M45" s="30"/>
+      <c r="M45" s="46"/>
     </row>
     <row r="46" spans="1:13" ht="16.5" customHeight="1">
       <c r="A46" s="12" t="s">
@@ -2130,12 +2130,12 @@
       <c r="I46" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J46" s="31" t="s">
+      <c r="J46" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="30"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="48"/>
+      <c r="M46" s="46"/>
     </row>
     <row r="47" spans="1:13" ht="16.5" customHeight="1">
       <c r="A47" s="12" t="s">
@@ -2149,14 +2149,14 @@
       <c r="E47" s="17"/>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
-      <c r="H47" s="48">
+      <c r="H47" s="36">
         <v>1000</v>
       </c>
-      <c r="I47" s="49"/>
+      <c r="I47" s="37"/>
       <c r="J47" s="17"/>
       <c r="K47" s="17"/>
       <c r="L47" s="17"/>
-      <c r="M47" s="30"/>
+      <c r="M47" s="46"/>
     </row>
     <row r="48" spans="1:13" ht="16.5" customHeight="1">
       <c r="A48" s="12" t="s">
@@ -2170,14 +2170,14 @@
       <c r="E48" s="17"/>
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
-      <c r="H48" s="48">
+      <c r="H48" s="36">
         <v>500</v>
       </c>
-      <c r="I48" s="49"/>
+      <c r="I48" s="37"/>
       <c r="J48" s="17"/>
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
-      <c r="M48" s="30"/>
+      <c r="M48" s="46"/>
     </row>
     <row r="49" spans="1:13" ht="16.5" customHeight="1">
       <c r="A49" s="13" t="s">
@@ -2191,14 +2191,14 @@
       <c r="E49" s="17"/>
       <c r="F49" s="17"/>
       <c r="G49" s="17"/>
-      <c r="H49" s="48">
+      <c r="H49" s="36">
         <v>100</v>
       </c>
-      <c r="I49" s="49"/>
+      <c r="I49" s="37"/>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
       <c r="L49" s="17"/>
-      <c r="M49" s="30"/>
+      <c r="M49" s="46"/>
     </row>
     <row r="50" spans="1:13" ht="16.5" customHeight="1">
       <c r="A50" s="13" t="s">
@@ -2212,14 +2212,14 @@
       <c r="E50" s="17"/>
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
-      <c r="H50" s="48">
+      <c r="H50" s="36">
         <v>50</v>
       </c>
-      <c r="I50" s="49"/>
+      <c r="I50" s="37"/>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
       <c r="L50" s="17"/>
-      <c r="M50" s="30"/>
+      <c r="M50" s="46"/>
     </row>
     <row r="51" spans="1:13" ht="16.5" customHeight="1">
       <c r="A51" s="13" t="s">
@@ -2233,14 +2233,14 @@
       <c r="E51" s="17"/>
       <c r="F51" s="17"/>
       <c r="G51" s="17"/>
-      <c r="H51" s="48">
+      <c r="H51" s="36">
         <v>20</v>
       </c>
-      <c r="I51" s="49"/>
+      <c r="I51" s="37"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
       <c r="L51" s="17"/>
-      <c r="M51" s="30"/>
+      <c r="M51" s="46"/>
     </row>
     <row r="52" spans="1:13" ht="16.5" customHeight="1">
       <c r="A52" s="13" t="s">
@@ -2254,14 +2254,14 @@
       <c r="E52" s="17"/>
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
-      <c r="H52" s="48">
+      <c r="H52" s="36">
         <v>10</v>
       </c>
-      <c r="I52" s="49"/>
+      <c r="I52" s="37"/>
       <c r="J52" s="17"/>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
-      <c r="M52" s="30"/>
+      <c r="M52" s="46"/>
     </row>
     <row r="53" spans="1:13" ht="16.5" customHeight="1">
       <c r="A53" s="13" t="s">
@@ -2275,14 +2275,14 @@
       <c r="E53" s="17"/>
       <c r="F53" s="17"/>
       <c r="G53" s="17"/>
-      <c r="H53" s="48">
+      <c r="H53" s="36">
         <v>5</v>
       </c>
-      <c r="I53" s="49"/>
+      <c r="I53" s="37"/>
       <c r="J53" s="17"/>
       <c r="K53" s="17"/>
       <c r="L53" s="17"/>
-      <c r="M53" s="30"/>
+      <c r="M53" s="46"/>
     </row>
     <row r="54" spans="1:13" ht="16.5" customHeight="1">
       <c r="A54" s="13" t="s">
@@ -2296,14 +2296,14 @@
       <c r="E54" s="17"/>
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
-      <c r="H54" s="48">
+      <c r="H54" s="36">
         <v>2</v>
       </c>
-      <c r="I54" s="49"/>
+      <c r="I54" s="37"/>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
-      <c r="M54" s="30"/>
+      <c r="M54" s="46"/>
     </row>
     <row r="55" spans="1:13" ht="16.5" customHeight="1">
       <c r="A55" s="12" t="s">
@@ -2324,88 +2324,88 @@
       <c r="J55" s="17"/>
       <c r="K55" s="17"/>
       <c r="L55" s="17"/>
-      <c r="M55" s="30"/>
+      <c r="M55" s="46"/>
     </row>
     <row r="56" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A56" s="34"/>
+      <c r="A56" s="28"/>
       <c r="B56" s="7"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="33"/>
-      <c r="I56" s="35"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="33"/>
-      <c r="L56" s="33"/>
-      <c r="M56" s="36"/>
+      <c r="C56" s="26"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
+      <c r="I56" s="29"/>
+      <c r="J56" s="26"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="27"/>
+      <c r="M56" s="30"/>
     </row>
     <row r="57" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A57" s="37" t="s">
+      <c r="A57" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="B57" s="38"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-      <c r="I57" s="35"/>
-      <c r="J57" s="32"/>
-      <c r="K57" s="33"/>
-      <c r="L57" s="33"/>
-      <c r="M57" s="39" t="s">
+      <c r="B57" s="40"/>
+      <c r="C57" s="26"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="29"/>
+      <c r="J57" s="26"/>
+      <c r="K57" s="27"/>
+      <c r="L57" s="27"/>
+      <c r="M57" s="31" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A58" s="38"/>
-      <c r="B58" s="38"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
-      <c r="H58" s="33"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="32"/>
-      <c r="K58" s="33"/>
-      <c r="L58" s="33"/>
-      <c r="M58" s="40"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="27"/>
+      <c r="E58" s="27"/>
+      <c r="F58" s="27"/>
+      <c r="G58" s="27"/>
+      <c r="H58" s="27"/>
+      <c r="I58" s="29"/>
+      <c r="J58" s="26"/>
+      <c r="K58" s="27"/>
+      <c r="L58" s="27"/>
+      <c r="M58" s="41"/>
     </row>
     <row r="59" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A59" s="38"/>
-      <c r="B59" s="38"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="33"/>
-      <c r="I59" s="35"/>
-      <c r="J59" s="32"/>
-      <c r="K59" s="33"/>
-      <c r="L59" s="33"/>
-      <c r="M59" s="40"/>
+      <c r="A59" s="40"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="27"/>
+      <c r="E59" s="27"/>
+      <c r="F59" s="27"/>
+      <c r="G59" s="27"/>
+      <c r="H59" s="27"/>
+      <c r="I59" s="29"/>
+      <c r="J59" s="26"/>
+      <c r="K59" s="27"/>
+      <c r="L59" s="27"/>
+      <c r="M59" s="41"/>
     </row>
     <row r="60" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A60" s="41" t="s">
+      <c r="A60" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="B60" s="41"/>
-      <c r="C60" s="32"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
-      <c r="H60" s="33"/>
-      <c r="I60" s="35"/>
-      <c r="J60" s="32"/>
-      <c r="K60" s="33"/>
-      <c r="L60" s="33"/>
-      <c r="M60" s="42" t="s">
+      <c r="B60" s="38"/>
+      <c r="C60" s="26"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="26"/>
+      <c r="K60" s="27"/>
+      <c r="L60" s="27"/>
+      <c r="M60" s="32" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
23.04.19 Today 6:03PM Sales Updated
</commit_message>
<xml_diff>
--- a/Othes/Allocation Sheet.xlsx
+++ b/Othes/Allocation Sheet.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Running" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Running!$A$5:$A$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Running!$A$5:$A$137</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Running!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="100">
   <si>
     <t>BL60</t>
   </si>
@@ -47,9 +47,6 @@
     <t>i60</t>
   </si>
   <si>
-    <t>Distributor Of Symphony (Mobile Hand Set)Edison Group</t>
-  </si>
-  <si>
     <t>Sales</t>
   </si>
   <si>
@@ -203,12 +200,6 @@
     <t>V94</t>
   </si>
   <si>
-    <t>Tulip-2</t>
-  </si>
-  <si>
-    <t>Madrasha Market Bagha Bazer , Rajshahi</t>
-  </si>
-  <si>
     <t>D54j</t>
   </si>
   <si>
@@ -317,7 +308,16 @@
     <t>v128</t>
   </si>
   <si>
-    <t>Date:22.04.19</t>
+    <t xml:space="preserve">Tulip-2 </t>
+  </si>
+  <si>
+    <t>Distributor Of Symphony (Mobile Hand Set) Edison Group</t>
+  </si>
+  <si>
+    <t>Date:23.04.19</t>
+  </si>
+  <si>
+    <t>Madrasha Market , Bagha Bazar , Bagha , Rajshahi</t>
   </si>
 </sst>
 </file>
@@ -327,7 +327,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -475,8 +475,15 @@
       <name val="Bauhaus 93"/>
       <family val="5"/>
     </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Bauhaus 93"/>
+      <family val="5"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -495,8 +502,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -541,13 +554,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -661,9 +689,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -678,6 +703,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -696,13 +730,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>29158</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>9720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>11308</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -740,13 +774,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>19439</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>1039975</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>1588</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1068,13 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:S134"/>
+  <dimension ref="A1:S135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection sqref="A1:M61"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="12.75"/>
@@ -1093,9 +1124,9 @@
     <col min="14" max="16384" width="20.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="23.25" customHeight="1">
-      <c r="A1" s="42" t="s">
-        <v>61</v>
+    <row r="1" spans="1:19" ht="33" customHeight="1">
+      <c r="A1" s="50" t="s">
+        <v>96</v>
       </c>
       <c r="B1" s="42"/>
       <c r="C1" s="42"/>
@@ -1118,7 +1149,7 @@
     </row>
     <row r="2" spans="1:19" ht="16.5" customHeight="1">
       <c r="A2" s="43" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
@@ -1141,7 +1172,7 @@
     </row>
     <row r="3" spans="1:19" ht="18.75" customHeight="1">
       <c r="A3" s="44" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
@@ -1163,21 +1194,21 @@
       <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A4" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
+      <c r="A4" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="52"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
+      <c r="K4" s="51"/>
+      <c r="L4" s="51"/>
+      <c r="M4" s="51"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
@@ -1187,46 +1218,46 @@
     </row>
     <row r="5" spans="1:19" ht="16.5" customHeight="1" thickTop="1">
       <c r="A5" s="23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="24" t="s">
-        <v>11</v>
-      </c>
       <c r="F5" s="24" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G5" s="24"/>
       <c r="H5" s="23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K5" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="24" t="s">
-        <v>11</v>
-      </c>
       <c r="M5" s="24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="16.5" customHeight="1">
       <c r="A6" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="18">
         <v>800</v>
@@ -1237,7 +1268,7 @@
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
       <c r="H6" s="34" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="I6" s="14">
         <v>7490</v>
@@ -1260,7 +1291,7 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="35" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I7" s="20">
         <v>8340</v>
@@ -1272,7 +1303,7 @@
     </row>
     <row r="8" spans="1:19" ht="16.5" customHeight="1">
       <c r="A8" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="18">
         <v>810</v>
@@ -1283,7 +1314,7 @@
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I8" s="12">
         <v>9190</v>
@@ -1295,7 +1326,7 @@
     </row>
     <row r="9" spans="1:19" ht="16.5" customHeight="1">
       <c r="A9" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B9" s="18">
         <v>800</v>
@@ -1306,7 +1337,7 @@
       <c r="F9" s="17"/>
       <c r="G9" s="17"/>
       <c r="H9" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="14">
         <v>3560</v>
@@ -1318,7 +1349,7 @@
     </row>
     <row r="10" spans="1:19" ht="16.5" customHeight="1">
       <c r="A10" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="18">
         <v>795</v>
@@ -1329,7 +1360,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="17"/>
       <c r="H10" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I10" s="14">
         <v>3340</v>
@@ -1341,7 +1372,7 @@
     </row>
     <row r="11" spans="1:19" ht="16.5" customHeight="1">
       <c r="A11" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="18">
         <v>790</v>
@@ -1352,7 +1383,7 @@
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
       <c r="H11" s="35" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="I11" s="14">
         <v>4690</v>
@@ -1375,7 +1406,7 @@
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
       <c r="H12" s="12" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I12" s="14">
         <v>5390</v>
@@ -1387,7 +1418,7 @@
     </row>
     <row r="13" spans="1:19" ht="16.5" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B13" s="18">
         <v>910</v>
@@ -1398,7 +1429,7 @@
       <c r="F13" s="17"/>
       <c r="G13" s="17"/>
       <c r="H13" s="34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I13" s="14">
         <v>4970</v>
@@ -1410,7 +1441,7 @@
     </row>
     <row r="14" spans="1:19" ht="16.5" customHeight="1">
       <c r="A14" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="18">
         <v>890</v>
@@ -1421,7 +1452,7 @@
       <c r="F14" s="17"/>
       <c r="G14" s="17"/>
       <c r="H14" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I14" s="14">
         <v>3710</v>
@@ -1444,7 +1475,7 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
       <c r="H15" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I15" s="14">
         <v>3620</v>
@@ -1456,7 +1487,7 @@
     </row>
     <row r="16" spans="1:19" ht="16.5" customHeight="1">
       <c r="A16" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="18">
         <v>880</v>
@@ -1467,7 +1498,7 @@
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
       <c r="H16" s="34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I16" s="14">
         <v>4620</v>
@@ -1479,7 +1510,7 @@
     </row>
     <row r="17" spans="1:13" ht="16.5" customHeight="1">
       <c r="A17" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B17" s="18">
         <v>1010</v>
@@ -1490,7 +1521,7 @@
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
       <c r="H17" s="21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I17" s="14">
         <v>4520</v>
@@ -1502,7 +1533,7 @@
     </row>
     <row r="18" spans="1:13" ht="16.5" customHeight="1">
       <c r="A18" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="18">
         <v>970</v>
@@ -1513,7 +1544,7 @@
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
       <c r="H18" s="21" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I18" s="14">
         <v>4080</v>
@@ -1536,7 +1567,7 @@
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
       <c r="H19" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I19" s="14">
         <v>4360</v>
@@ -1559,7 +1590,7 @@
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
       <c r="H20" s="21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="I20" s="14">
         <v>4640</v>
@@ -1571,10 +1602,10 @@
     </row>
     <row r="21" spans="1:13" ht="16.5" customHeight="1">
       <c r="A21" s="12" t="s">
-        <v>64</v>
+        <v>1</v>
       </c>
       <c r="B21" s="18">
-        <v>1000</v>
+        <v>995</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -1582,7 +1613,7 @@
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
       <c r="H21" s="21" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I21" s="14">
         <v>4640</v>
@@ -1594,10 +1625,10 @@
     </row>
     <row r="22" spans="1:13" ht="16.5" customHeight="1">
       <c r="A22" s="12" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B22" s="18">
-        <v>960</v>
+        <v>1000</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -1605,7 +1636,7 @@
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
       <c r="H22" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I22" s="14">
         <v>5650</v>
@@ -1617,10 +1648,10 @@
     </row>
     <row r="23" spans="1:13" ht="16.5" customHeight="1">
       <c r="A23" s="12" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B23" s="18">
-        <v>980</v>
+        <v>960</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -1628,7 +1659,7 @@
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I23" s="14">
         <v>5020</v>
@@ -1640,10 +1671,10 @@
     </row>
     <row r="24" spans="1:13" ht="16.5" customHeight="1">
       <c r="A24" s="12" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B24" s="18">
-        <v>1040</v>
+        <v>980</v>
       </c>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -1651,7 +1682,7 @@
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
       <c r="H24" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I24" s="14">
         <v>5280</v>
@@ -1663,10 +1694,10 @@
     </row>
     <row r="25" spans="1:13" ht="16.5" customHeight="1">
       <c r="A25" s="12" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B25" s="18">
-        <v>1290</v>
+        <v>1040</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -1674,7 +1705,7 @@
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
       <c r="H25" s="21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I25" s="14">
         <v>5440</v>
@@ -1689,7 +1720,7 @@
         <v>63</v>
       </c>
       <c r="B26" s="18">
-        <v>1270</v>
+        <v>1290</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -1697,7 +1728,7 @@
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
       <c r="H26" s="21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I26" s="14">
         <v>5560</v>
@@ -1709,18 +1740,18 @@
     </row>
     <row r="27" spans="1:13" ht="16.5" customHeight="1">
       <c r="A27" s="12" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="B27" s="18">
-        <v>1190</v>
+        <v>1270</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
-      <c r="H27" s="35" t="s">
-        <v>58</v>
+      <c r="H27" s="21" t="s">
+        <v>57</v>
       </c>
       <c r="I27" s="14">
         <v>6090</v>
@@ -1732,10 +1763,10 @@
     </row>
     <row r="28" spans="1:13" ht="16.5" customHeight="1">
       <c r="A28" s="12" t="s">
-        <v>67</v>
+        <v>24</v>
       </c>
       <c r="B28" s="18">
-        <v>1290</v>
+        <v>1190</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -1743,7 +1774,7 @@
       <c r="F28" s="17"/>
       <c r="G28" s="17"/>
       <c r="H28" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I28" s="14">
         <v>5390</v>
@@ -1755,20 +1786,20 @@
     </row>
     <row r="29" spans="1:13" ht="16.5" customHeight="1">
       <c r="A29" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B29" s="18">
-        <v>1190</v>
+        <v>1290</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="17"/>
       <c r="G29" s="17"/>
-      <c r="H29" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="I29" s="20">
+      <c r="H29" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" s="14">
         <v>12590</v>
       </c>
       <c r="J29" s="17"/>
@@ -1778,18 +1809,18 @@
     </row>
     <row r="30" spans="1:13" ht="16.5" customHeight="1">
       <c r="A30" s="12" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="B30" s="18">
-        <v>1080</v>
+        <v>1190</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
-      <c r="H30" s="34" t="s">
-        <v>83</v>
+      <c r="H30" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="I30" s="20">
         <v>12240</v>
@@ -1801,10 +1832,10 @@
     </row>
     <row r="31" spans="1:13" ht="16.5" customHeight="1">
       <c r="A31" s="12" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B31" s="18">
-        <v>1100</v>
+        <v>1080</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -1812,7 +1843,7 @@
       <c r="F31" s="17"/>
       <c r="G31" s="17"/>
       <c r="H31" s="34" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I31" s="20">
         <v>12090</v>
@@ -1824,10 +1855,10 @@
     </row>
     <row r="32" spans="1:13" ht="16.5" customHeight="1">
       <c r="A32" s="12" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B32" s="18">
-        <v>1120</v>
+        <v>1100</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
@@ -1835,9 +1866,9 @@
       <c r="F32" s="17"/>
       <c r="G32" s="17"/>
       <c r="H32" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="I32" s="14">
+        <v>82</v>
+      </c>
+      <c r="I32" s="20">
         <v>10840</v>
       </c>
       <c r="J32" s="17"/>
@@ -1847,20 +1878,20 @@
     </row>
     <row r="33" spans="1:13" ht="16.5" customHeight="1">
       <c r="A33" s="12" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B33" s="18">
-        <v>1040</v>
+        <v>1120</v>
       </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
       <c r="F33" s="17"/>
       <c r="G33" s="17"/>
-      <c r="H33" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="I33" s="20">
+      <c r="H33" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="I33" s="14">
         <v>12490</v>
       </c>
       <c r="J33" s="17"/>
@@ -1870,20 +1901,20 @@
     </row>
     <row r="34" spans="1:13" ht="16.5" customHeight="1">
       <c r="A34" s="12" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B34" s="18">
-        <v>1100</v>
+        <v>1040</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
       <c r="F34" s="17"/>
       <c r="G34" s="17"/>
-      <c r="H34" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="I34" s="14">
+      <c r="H34" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="I34" s="20">
         <v>12800</v>
       </c>
       <c r="J34" s="17"/>
@@ -1893,9 +1924,9 @@
     </row>
     <row r="35" spans="1:13" ht="16.5" customHeight="1">
       <c r="A35" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="19">
+        <v>46</v>
+      </c>
+      <c r="B35" s="18">
         <v>1100</v>
       </c>
       <c r="C35" s="17"/>
@@ -1903,8 +1934,8 @@
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
       <c r="G35" s="17"/>
-      <c r="H35" s="34" t="s">
-        <v>88</v>
+      <c r="H35" s="21" t="s">
+        <v>85</v>
       </c>
       <c r="I35" s="14">
         <v>17790</v>
@@ -1916,10 +1947,10 @@
     </row>
     <row r="36" spans="1:13" ht="16.5" customHeight="1">
       <c r="A36" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B36" s="18">
-        <v>1130</v>
+        <v>7</v>
+      </c>
+      <c r="B36" s="19">
+        <v>1100</v>
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
@@ -1927,7 +1958,7 @@
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
       <c r="H36" s="34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="I36" s="14">
         <v>7740</v>
@@ -1939,10 +1970,10 @@
     </row>
     <row r="37" spans="1:13" ht="16.5" customHeight="1">
       <c r="A37" s="12" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B37" s="18">
-        <v>1100</v>
+        <v>1130</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17"/>
@@ -1958,10 +1989,10 @@
     </row>
     <row r="38" spans="1:13" ht="16.5" customHeight="1">
       <c r="A38" s="12" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="B38" s="18">
-        <v>1330</v>
+        <v>1100</v>
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
@@ -1977,7 +2008,7 @@
     </row>
     <row r="39" spans="1:13" ht="16.5" customHeight="1">
       <c r="A39" s="12" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B39" s="18">
         <v>1330</v>
@@ -1987,8 +2018,8 @@
       <c r="E39" s="17"/>
       <c r="F39" s="17"/>
       <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="20"/>
+      <c r="H39" s="34"/>
+      <c r="I39" s="14"/>
       <c r="J39" s="17"/>
       <c r="K39" s="17"/>
       <c r="L39" s="17"/>
@@ -1996,18 +2027,18 @@
     </row>
     <row r="40" spans="1:13" ht="16.5" customHeight="1">
       <c r="A40" s="12" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B40" s="18">
-        <v>1200</v>
+        <v>1330</v>
       </c>
       <c r="C40" s="17"/>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
       <c r="F40" s="17"/>
       <c r="G40" s="17"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="14"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="20"/>
       <c r="J40" s="17"/>
       <c r="K40" s="17"/>
       <c r="L40" s="17"/>
@@ -2015,10 +2046,10 @@
     </row>
     <row r="41" spans="1:13" ht="16.5" customHeight="1">
       <c r="A41" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B41" s="18">
-        <v>1220</v>
+        <v>1200</v>
       </c>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
@@ -2034,10 +2065,10 @@
     </row>
     <row r="42" spans="1:13" ht="16.5" customHeight="1">
       <c r="A42" s="12" t="s">
-        <v>77</v>
+        <v>32</v>
       </c>
       <c r="B42" s="18">
-        <v>1460</v>
+        <v>1220</v>
       </c>
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
@@ -2053,117 +2084,115 @@
     </row>
     <row r="43" spans="1:13" ht="16.5" customHeight="1">
       <c r="A43" s="12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B43" s="18">
-        <v>1470</v>
+        <v>1460</v>
       </c>
       <c r="C43" s="17"/>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
       <c r="G43" s="17"/>
-      <c r="H43" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="I43" s="50"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="49"/>
-      <c r="L43" s="49"/>
-      <c r="M43" s="33"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
     </row>
     <row r="44" spans="1:13" ht="16.5" customHeight="1">
       <c r="A44" s="12" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B44" s="18">
-        <v>1590</v>
+        <v>1470</v>
       </c>
       <c r="C44" s="17"/>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
-      <c r="H44" s="49"/>
+      <c r="H44" s="48" t="s">
+        <v>17</v>
+      </c>
       <c r="I44" s="49"/>
-      <c r="J44" s="49"/>
-      <c r="K44" s="49"/>
-      <c r="L44" s="49"/>
-      <c r="M44" s="49"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="48"/>
+      <c r="L44" s="48"/>
+      <c r="M44" s="33"/>
     </row>
     <row r="45" spans="1:13" ht="16.5" customHeight="1">
       <c r="A45" s="12" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B45" s="18">
-        <v>1480</v>
+        <v>1590</v>
       </c>
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
       <c r="G45" s="17"/>
-      <c r="H45" s="47" t="s">
-        <v>14</v>
-      </c>
-      <c r="I45" s="47"/>
-      <c r="J45" s="47"/>
-      <c r="K45" s="47"/>
-      <c r="L45" s="47"/>
-      <c r="M45" s="46"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="48"/>
     </row>
     <row r="46" spans="1:13" ht="16.5" customHeight="1">
       <c r="A46" s="12" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="B46" s="18">
-        <v>1730</v>
+        <v>1480</v>
       </c>
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
       <c r="G46" s="17"/>
-      <c r="H46" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I46" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J46" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="K46" s="48"/>
-      <c r="L46" s="48"/>
-      <c r="M46" s="46"/>
+      <c r="H46" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" s="46"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
+      <c r="L46" s="46"/>
+      <c r="M46" s="45"/>
     </row>
     <row r="47" spans="1:13" ht="16.5" customHeight="1">
       <c r="A47" s="12" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B47" s="18">
-        <v>1250</v>
+        <v>1730</v>
       </c>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
       <c r="F47" s="17"/>
       <c r="G47" s="17"/>
-      <c r="H47" s="36">
-        <v>1000</v>
-      </c>
-      <c r="I47" s="37"/>
-      <c r="J47" s="17"/>
-      <c r="K47" s="17"/>
-      <c r="L47" s="17"/>
-      <c r="M47" s="46"/>
+      <c r="H47" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I47" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="K47" s="47"/>
+      <c r="L47" s="47"/>
+      <c r="M47" s="45"/>
     </row>
     <row r="48" spans="1:13" ht="16.5" customHeight="1">
       <c r="A48" s="12" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B48" s="18">
-        <v>1370</v>
+        <v>1250</v>
       </c>
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
@@ -2171,20 +2200,20 @@
       <c r="F48" s="17"/>
       <c r="G48" s="17"/>
       <c r="H48" s="36">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="I48" s="37"/>
       <c r="J48" s="17"/>
       <c r="K48" s="17"/>
       <c r="L48" s="17"/>
-      <c r="M48" s="46"/>
+      <c r="M48" s="45"/>
     </row>
     <row r="49" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A49" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" s="13">
-        <v>1890</v>
+      <c r="A49" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="18">
+        <v>1370</v>
       </c>
       <c r="C49" s="17"/>
       <c r="D49" s="17"/>
@@ -2192,20 +2221,20 @@
       <c r="F49" s="17"/>
       <c r="G49" s="17"/>
       <c r="H49" s="36">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="I49" s="37"/>
       <c r="J49" s="17"/>
       <c r="K49" s="17"/>
       <c r="L49" s="17"/>
-      <c r="M49" s="46"/>
+      <c r="M49" s="45"/>
     </row>
     <row r="50" spans="1:13" ht="16.5" customHeight="1">
       <c r="A50" s="13" t="s">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="B50" s="13">
-        <v>2780</v>
+        <v>1890</v>
       </c>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
@@ -2213,20 +2242,20 @@
       <c r="F50" s="17"/>
       <c r="G50" s="17"/>
       <c r="H50" s="36">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I50" s="37"/>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
       <c r="L50" s="17"/>
-      <c r="M50" s="46"/>
+      <c r="M50" s="45"/>
     </row>
     <row r="51" spans="1:13" ht="16.5" customHeight="1">
       <c r="A51" s="13" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="B51" s="13">
-        <v>6540</v>
+        <v>2780</v>
       </c>
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
@@ -2234,20 +2263,20 @@
       <c r="F51" s="17"/>
       <c r="G51" s="17"/>
       <c r="H51" s="36">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="I51" s="37"/>
       <c r="J51" s="17"/>
       <c r="K51" s="17"/>
       <c r="L51" s="17"/>
-      <c r="M51" s="46"/>
+      <c r="M51" s="45"/>
     </row>
     <row r="52" spans="1:13" ht="16.5" customHeight="1">
       <c r="A52" s="13" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B52" s="13">
-        <v>6210</v>
+        <v>6540</v>
       </c>
       <c r="C52" s="17"/>
       <c r="D52" s="17"/>
@@ -2255,20 +2284,20 @@
       <c r="F52" s="17"/>
       <c r="G52" s="17"/>
       <c r="H52" s="36">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I52" s="37"/>
       <c r="J52" s="17"/>
       <c r="K52" s="17"/>
       <c r="L52" s="17"/>
-      <c r="M52" s="46"/>
+      <c r="M52" s="45"/>
     </row>
     <row r="53" spans="1:13" ht="16.5" customHeight="1">
       <c r="A53" s="13" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B53" s="13">
-        <v>7075</v>
+        <v>6210</v>
       </c>
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
@@ -2276,20 +2305,20 @@
       <c r="F53" s="17"/>
       <c r="G53" s="17"/>
       <c r="H53" s="36">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I53" s="37"/>
       <c r="J53" s="17"/>
       <c r="K53" s="17"/>
       <c r="L53" s="17"/>
-      <c r="M53" s="46"/>
+      <c r="M53" s="45"/>
     </row>
     <row r="54" spans="1:13" ht="16.5" customHeight="1">
       <c r="A54" s="13" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="B54" s="13">
-        <v>7910</v>
+        <v>7075</v>
       </c>
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>
@@ -2297,55 +2326,59 @@
       <c r="F54" s="17"/>
       <c r="G54" s="17"/>
       <c r="H54" s="36">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I54" s="37"/>
       <c r="J54" s="17"/>
       <c r="K54" s="17"/>
       <c r="L54" s="17"/>
-      <c r="M54" s="46"/>
+      <c r="M54" s="45"/>
     </row>
     <row r="55" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A55" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="B55" s="12">
-        <v>7890</v>
-      </c>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
+      <c r="A55" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" s="13">
+        <v>7910</v>
+      </c>
+      <c r="C55" s="17"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="17"/>
       <c r="F55" s="17"/>
       <c r="G55" s="17"/>
-      <c r="H55" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="I55" s="17"/>
+      <c r="H55" s="36">
+        <v>2</v>
+      </c>
+      <c r="I55" s="37"/>
       <c r="J55" s="17"/>
       <c r="K55" s="17"/>
       <c r="L55" s="17"/>
-      <c r="M55" s="46"/>
+      <c r="M55" s="45"/>
     </row>
     <row r="56" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A56" s="28"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="29"/>
-      <c r="J56" s="26"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="30"/>
+      <c r="A56" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="12">
+        <v>7890</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="45"/>
     </row>
     <row r="57" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A57" s="39" t="s">
-        <v>93</v>
-      </c>
-      <c r="B57" s="40"/>
+      <c r="A57" s="28"/>
+      <c r="B57" s="7"/>
       <c r="C57" s="26"/>
       <c r="D57" s="27"/>
       <c r="E57" s="27"/>
@@ -2356,12 +2389,12 @@
       <c r="J57" s="26"/>
       <c r="K57" s="27"/>
       <c r="L57" s="27"/>
-      <c r="M57" s="31" t="s">
-        <v>96</v>
-      </c>
+      <c r="M57" s="30"/>
     </row>
     <row r="58" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A58" s="40"/>
+      <c r="A58" s="39" t="s">
+        <v>90</v>
+      </c>
       <c r="B58" s="40"/>
       <c r="C58" s="26"/>
       <c r="D58" s="27"/>
@@ -2373,7 +2406,9 @@
       <c r="J58" s="26"/>
       <c r="K58" s="27"/>
       <c r="L58" s="27"/>
-      <c r="M58" s="41"/>
+      <c r="M58" s="31" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="59" spans="1:13" ht="16.5" customHeight="1">
       <c r="A59" s="40"/>
@@ -2391,10 +2426,8 @@
       <c r="M59" s="41"/>
     </row>
     <row r="60" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A60" s="38" t="s">
-        <v>94</v>
-      </c>
-      <c r="B60" s="38"/>
+      <c r="A60" s="40"/>
+      <c r="B60" s="40"/>
       <c r="C60" s="26"/>
       <c r="D60" s="27"/>
       <c r="E60" s="27"/>
@@ -2405,15 +2438,31 @@
       <c r="J60" s="26"/>
       <c r="K60" s="27"/>
       <c r="L60" s="27"/>
-      <c r="M60" s="32" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="16.5" customHeight="1"/>
-    <row r="62" spans="1:13" ht="16.5" customHeight="1">
-      <c r="G62" s="11"/>
-    </row>
-    <row r="63" spans="1:13" ht="16.5" customHeight="1"/>
+      <c r="M60" s="41"/>
+    </row>
+    <row r="61" spans="1:13" ht="16.5" customHeight="1">
+      <c r="A61" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" s="38"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="27"/>
+      <c r="L61" s="27"/>
+      <c r="M61" s="32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" ht="16.5" customHeight="1"/>
+    <row r="63" spans="1:13" ht="16.5" customHeight="1">
+      <c r="G63" s="11"/>
+    </row>
     <row r="64" spans="1:13" ht="16.5" customHeight="1"/>
     <row r="65" ht="16.5" customHeight="1"/>
     <row r="66" ht="16.5" customHeight="1"/>
@@ -2427,7 +2476,7 @@
     <row r="74" ht="16.5" customHeight="1"/>
     <row r="75" ht="16.5" customHeight="1"/>
     <row r="76" ht="16.5" customHeight="1"/>
-    <row r="77" ht="15" customHeight="1"/>
+    <row r="77" ht="16.5" customHeight="1"/>
     <row r="78" ht="15" customHeight="1"/>
     <row r="79" ht="15" customHeight="1"/>
     <row r="80" ht="15" customHeight="1"/>
@@ -2455,10 +2504,10 @@
     <row r="102" spans="3:3" ht="15" customHeight="1"/>
     <row r="103" spans="3:3" ht="15" customHeight="1"/>
     <row r="104" spans="3:3" ht="15" customHeight="1"/>
-    <row r="105" spans="3:3" ht="15" customHeight="1">
-      <c r="C105" s="10"/>
-    </row>
-    <row r="106" spans="3:3" ht="15" customHeight="1"/>
+    <row r="105" spans="3:3" ht="15" customHeight="1"/>
+    <row r="106" spans="3:3" ht="15" customHeight="1">
+      <c r="C106" s="10"/>
+    </row>
     <row r="107" spans="3:3" ht="15" customHeight="1"/>
     <row r="108" spans="3:3" ht="15" customHeight="1"/>
     <row r="109" spans="3:3" ht="15" customHeight="1"/>
@@ -2487,26 +2536,26 @@
     <row r="132" ht="15" customHeight="1"/>
     <row r="133" ht="15" customHeight="1"/>
     <row r="134" ht="15" customHeight="1"/>
+    <row r="135" ht="15" customHeight="1"/>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B59"/>
-    <mergeCell ref="M58:M59"/>
+  <mergeCells count="13">
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B60"/>
+    <mergeCell ref="M59:M60"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:M4"/>
-    <mergeCell ref="M45:M55"/>
-    <mergeCell ref="H45:L45"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="H44:M44"/>
+    <mergeCell ref="M46:M56"/>
+    <mergeCell ref="H46:L46"/>
+    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="H45:M45"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="83" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0.5" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
30.04.19 Sales Updated 6:29PM
</commit_message>
<xml_diff>
--- a/Othes/Allocation Sheet.xlsx
+++ b/Othes/Allocation Sheet.xlsx
@@ -320,7 +320,7 @@
     <t>L250</t>
   </si>
   <si>
-    <t>Date:28.04.19</t>
+    <t>Date:30.04.19</t>
   </si>
 </sst>
 </file>
@@ -1108,7 +1108,7 @@
   <dimension ref="A1:S135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection sqref="A1:M61"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="12.75"/>

</xml_diff>